<commit_message>
Update to include comparators and predicate search.
</commit_message>
<xml_diff>
--- a/WebContent/assets/spreadsheets/Movies.xlsx
+++ b/WebContent/assets/spreadsheets/Movies.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\files\development\workspace\Movies_dpope3\WebContent\assets\spreadsheets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="940" windowWidth="25600" windowHeight="14620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12090" windowHeight="3310"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Rope</t>
   </si>
@@ -44,6 +40,12 @@
   </si>
   <si>
     <t>Ingmar Bergman</t>
+  </si>
+  <si>
+    <t>Goodfellas</t>
+  </si>
+  <si>
+    <t>Martin Scorsese</t>
   </si>
 </sst>
 </file>
@@ -385,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -433,6 +435,17 @@
         <v>96</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>